<commit_message>
Checkout addrress verification added
</commit_message>
<xml_diff>
--- a/testdata/Book2.xlsx
+++ b/testdata/Book2.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowHeight="12090" windowWidth="25875" xWindow="1230" yWindow="-105"/>
+    <workbookView activeTab="1" windowHeight="12090" windowWidth="25875" xWindow="2085" yWindow="255"/>
   </bookViews>
   <sheets>
     <sheet name="Qty" r:id="rId1" sheetId="1"/>
-    <sheet name="Sheet2" r:id="rId2" sheetId="2"/>
+    <sheet name="Address" r:id="rId2" sheetId="2"/>
     <sheet name="Sheet3" r:id="rId3" sheetId="3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="34">
   <si>
     <t>qty</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Success: You have added HP LP3065 to your shopping cart!</t>
   </si>
   <si>
-    <t>Abc</t>
-  </si>
-  <si>
     <t>-45</t>
   </si>
   <si>
@@ -51,36 +48,15 @@
     <t>Failed</t>
   </si>
   <si>
-    <t>-46</t>
-  </si>
-  <si>
-    <t>-48</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
-    <t>hyrt</t>
-  </si>
-  <si>
-    <t>aswd</t>
-  </si>
-  <si>
     <t>SDD</t>
   </si>
   <si>
-    <t>-1</t>
-  </si>
-  <si>
     <t>Passed</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
     <t>25</t>
   </si>
   <si>
@@ -93,7 +69,55 @@
     <t>4</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>Hold</t>
+  </si>
+  <si>
+    <t>first</t>
+  </si>
+  <si>
+    <t>last</t>
+  </si>
+  <si>
+    <t>address1</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>pincode</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Vivek</t>
+  </si>
+  <si>
+    <t>Ingole</t>
+  </si>
+  <si>
+    <t>Hinjewadi Phase 3</t>
+  </si>
+  <si>
+    <t>Pune</t>
+  </si>
+  <si>
+    <t>413309</t>
+  </si>
+  <si>
+    <t>107</t>
+  </si>
+  <si>
+    <t>19</t>
   </si>
 </sst>
 </file>
@@ -145,7 +169,50 @@
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
@@ -435,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -459,59 +526,45 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1"/>
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>25</v>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="3" t="s">
-        <v>19</v>
+      <c r="A3" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>25</v>
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -521,196 +574,347 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B23:E43"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" customWidth="true" width="22.140625" collapsed="true"/>
+  </cols>
   <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="B5" s="3"/>
+      <c r="D5" s="2"/>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="B6" s="3"/>
+      <c r="D6" s="2"/>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="B7" s="3"/>
+      <c r="D7" s="2"/>
+      <c r="G7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="B8" s="3"/>
+      <c r="D8" s="2"/>
+      <c r="G8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="B9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="G9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="B10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="G10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="B11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="G11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="B12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="G12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="B13" s="3"/>
+      <c r="D13" s="2"/>
+      <c r="G13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="B14" s="3"/>
+      <c r="D14" s="2"/>
+      <c r="G14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="B15" s="3"/>
+      <c r="D15" s="2"/>
+      <c r="G15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="B16" s="3"/>
+      <c r="D16" s="2"/>
+      <c r="G16" t="s">
+        <v>18</v>
+      </c>
+    </row>
     <row r="23" spans="2:4">
       <c r="B23" s="1"/>
-      <c r="C23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>3</v>
+      <c r="D23" s="1"/>
+      <c r="G23" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" s="1"/>
-      <c r="C24" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>3</v>
+      <c r="D24" s="1"/>
+      <c r="G24" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="2:4">
       <c r="B25" s="1"/>
-      <c r="C25" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>3</v>
+      <c r="D25" s="1"/>
+      <c r="G25" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="2:4">
-      <c r="B26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>4</v>
+      <c r="B26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="G26" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="2:4">
-      <c r="B27" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>4</v>
+      <c r="B27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="G27" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="2:4">
-      <c r="B28" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>4</v>
+      <c r="B28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="G28" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="2:4">
-      <c r="B29" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>4</v>
+      <c r="B29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="G29" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="2:4">
-      <c r="B30" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>5</v>
+      <c r="B30" s="3"/>
+      <c r="D30" s="2"/>
+      <c r="G30" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="2:4">
-      <c r="B31" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C31" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>5</v>
+      <c r="B31" s="3"/>
+      <c r="D31" s="2"/>
+      <c r="G31" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="2:4">
-      <c r="B32" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>5</v>
+      <c r="B32" s="3"/>
+      <c r="D32" s="2"/>
+      <c r="G32" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="2:4">
-      <c r="B33" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C33" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>5</v>
+      <c r="B33" s="3"/>
+      <c r="D33" s="2"/>
+      <c r="G33" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="2:4">
       <c r="B38" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C38" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="G38" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="39" spans="2:4">
       <c r="B39" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C39" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="G39" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="40" spans="2:4">
       <c r="B40" s="3" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C40" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="G40" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="41" spans="2:4">
       <c r="B41" s="3" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C41" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="G41" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="42" spans="2:4">
       <c r="B42" s="3" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="G42" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="43" spans="2:4">
       <c r="B43" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="G43" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="H2:H3">
+    <cfRule dxfId="5" operator="equal" priority="2" stopIfTrue="1" type="cellIs">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule dxfId="4" operator="containsText" priority="3" stopIfTrue="1" text="Passed" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Passed",H2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H3">
+    <cfRule dxfId="1" operator="containsText" priority="1" stopIfTrue="1" text="Hold" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Hold",H2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="H2:H3" type="list">
+      <formula1>"Passed,Failed,Hold"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>

</xml_diff>